<commit_message>
create versioning of script : version 1.0
</commit_message>
<xml_diff>
--- a/XRayTracing_Input.xlsx
+++ b/XRayTracing_Input.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BAPAK\OneDrive - IBA Group\Documents\XRayTracing_script\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8CE9809-6683-43EC-8EF5-2DBC0AF4FBA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA77D8D-E2FE-4836-9046-D5D7976753D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset" sheetId="2" r:id="rId1"/>
+    <sheet name="Extra Info" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="81">
   <si>
     <t>Simulation number</t>
   </si>
@@ -273,13 +274,16 @@
   </si>
   <si>
     <t>[1.5, 1.5, 1.5, 1.25, 1.15, 1.07, 1.02, 0.98, 0.94, 0.91, 0.90, 0.91, 0.94, 0.98, 1.02, 1.07, 1.15, 1.25, 1.5, 1.5, 1.5]</t>
+  </si>
+  <si>
+    <t>Script Version 1.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,6 +307,13 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -747,7 +758,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -934,6 +945,24 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -955,62 +984,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="40">
-    <dxf>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="15" formatCode="0.00E+00"/>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -1441,6 +1420,54 @@
         <bottom/>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border outline="0">
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1543,40 +1570,40 @@
     <tableColumn id="47" xr3:uid="{00000000-0010-0000-0000-00002F000000}" name="Run (V or X)" dataDxfId="36"/>
     <tableColumn id="91" xr3:uid="{626FBC7C-3428-4D9C-8245-E9980AC00DE2}" name="Source X-dimension [cm]" dataDxfId="35"/>
     <tableColumn id="92" xr3:uid="{48847A7E-649C-495D-90D0-0688D87DF622}" name="Source Y-dimension [cm]" dataDxfId="34"/>
-    <tableColumn id="93" xr3:uid="{66149D7C-1A46-4A74-A17E-BAA01A3EF0E9}" name="Source resolution (X,Y,) [cm²]" dataDxfId="2"/>
-    <tableColumn id="101" xr3:uid="{AFAA355A-5088-4D32-864A-D3766E3F2DB9}" name="Variable Current in X direction [mA]" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{B8B68D9B-B8A5-47C6-9E38-96ACC38FEEBF}" name="Variable Current in Y direction [mA]" dataDxfId="1"/>
-    <tableColumn id="113" xr3:uid="{52A1E8D6-8081-4659-A014-60E4EF5F0E59}" name="Conveyor density [g/cm³]" dataDxfId="3"/>
-    <tableColumn id="94" xr3:uid="{96888CAA-C7C5-4E47-8448-9191C49FA5A1}" name="Conveyor dimensions [cm³]" dataDxfId="33"/>
-    <tableColumn id="95" xr3:uid="{ED0D4D0E-1211-43F2-BC0E-22DA81926893}" name="Conveyor (X,Z,) offset to source [cm]²" dataDxfId="32"/>
-    <tableColumn id="98" xr3:uid="{A2FC2080-D096-4223-A065-59BF125992CF}" name="Conveyor speed [m/min]" dataDxfId="31"/>
-    <tableColumn id="99" xr3:uid="{5E6C370D-3088-4624-AFB4-003F396975BF}" name="Operation [hours/year]" dataDxfId="30"/>
-    <tableColumn id="102" xr3:uid="{770C3078-401F-4D26-A1DF-66B2FFE02E8B}" name="Central product density [g/cm³]" dataDxfId="29"/>
-    <tableColumn id="48" xr3:uid="{CCB69289-CD76-4BD9-9335-F57431C42E63}" name="Central product dimensions [cm³]" dataDxfId="28"/>
-    <tableColumn id="107" xr3:uid="{7D836FFB-FB1E-4F92-B391-5A079FD28583}" name="Central product (Y,Z,) position [cm]" dataDxfId="27"/>
-    <tableColumn id="105" xr3:uid="{52C3BF51-271E-47F7-AA33-2A718B0AF70E}" name="Central product resolution (X,Y,Z) [cm³]" dataDxfId="26"/>
-    <tableColumn id="80" xr3:uid="{9673494C-D662-4EC2-81E7-43A6012DBA29}" name="Central wooden pallet density [g/cm³]" dataDxfId="25"/>
-    <tableColumn id="78" xr3:uid="{AD143500-9222-4D71-A52F-89788F0E51BF}" name="Central wooden pallet dimensions [cm³]" dataDxfId="24"/>
-    <tableColumn id="104" xr3:uid="{64CF5341-FD0F-4CC6-8051-EDE54CCFDAFD}" name="Left product density [g/cm³]" dataDxfId="23"/>
-    <tableColumn id="103" xr3:uid="{302258E3-A3C1-449E-A147-45DF85CD8461}" name="Left product dimensions [cm³]" dataDxfId="22"/>
-    <tableColumn id="81" xr3:uid="{F4817E2A-8E0A-4F71-AEEF-983CB4BA5C5A}" name="Left product Y-gap [cm]" dataDxfId="21"/>
-    <tableColumn id="79" xr3:uid="{D4890004-1BD6-47CE-A0AD-30515FDE1C89}" name="Left wooden pallet density [g/cm³]" dataDxfId="20"/>
-    <tableColumn id="49" xr3:uid="{99EDCD1E-4E84-4177-8AE8-B85A1112E226}" name="Left wooden pallet dimensions [cm³]" dataDxfId="19"/>
-    <tableColumn id="68" xr3:uid="{134833D5-3CD0-445F-96A6-F83F3F601C27}" name="Right product density [g/cm³]" dataDxfId="18"/>
-    <tableColumn id="69" xr3:uid="{57F245DA-9F77-4C92-89BD-07EC51E62BA7}" name="Right product dimensions [cm³]" dataDxfId="17"/>
-    <tableColumn id="85" xr3:uid="{872D630E-21C6-45BA-BF05-CA39F0614DE6}" name="Right product Y-gap [cm]" dataDxfId="16"/>
-    <tableColumn id="84" xr3:uid="{65B9F3CC-FE71-4DC2-B3A1-DCE7E9DFB044}" name="Right wooden pallet density [g/cm³]" dataDxfId="15"/>
-    <tableColumn id="83" xr3:uid="{C788756D-428F-464B-BB5B-33F86DA3B670}" name="Right wooden pallet dimensions [cm³]" dataDxfId="14"/>
-    <tableColumn id="82" xr3:uid="{F993C600-89C0-4209-8324-76E491F0FF21}" name="Mother pallets density [g/cm³]" dataDxfId="13"/>
-    <tableColumn id="65" xr3:uid="{E2839587-C22B-4C24-A46E-35133C720E5D}" name="Mother pallets dimensions [cm³]" dataDxfId="12"/>
-    <tableColumn id="75" xr3:uid="{D92D691F-4F6B-4EA0-8A3B-CC42AE83D3EB}" name="Units (Gy/h) (kGy/h) (Gy) (kGy)" dataDxfId="11"/>
-    <tableColumn id="63" xr3:uid="{EF6E5902-20A7-42BC-AA8A-69AFA6FA6571}" name="Minimum dose" dataDxfId="10"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Purpose of the test" dataDxfId="9"/>
-    <tableColumn id="77" xr3:uid="{95DD1121-A20B-405B-B9A1-FE5D35E618A0}" name="List of n 0-D dose mapping points (X1,Y1,Z1), …, (Xn,Yn,Zn)" dataDxfId="8"/>
-    <tableColumn id="109" xr3:uid="{EAC4DB55-B00A-46BE-AD00-296DD033D394}" name="X-mapping (V or X)" dataDxfId="7"/>
-    <tableColumn id="111" xr3:uid="{738EFEBD-DE05-475E-AAEA-A33A35B3E948}" name="Y-mapping (V or X)" dataDxfId="6"/>
-    <tableColumn id="110" xr3:uid="{DBF499A0-44D0-419A-909B-771F65574919}" name="Z-mapping (V or X)" dataDxfId="5"/>
-    <tableColumn id="90" xr3:uid="{59CF94CA-802D-4A0C-8D11-1660040EBEDD}" name="List of p 1-D mapping points (X1,Y1,Z1), …, (Xp,Yp,Zp)" dataDxfId="4"/>
+    <tableColumn id="93" xr3:uid="{66149D7C-1A46-4A74-A17E-BAA01A3EF0E9}" name="Source resolution (X,Y,) [cm²]" dataDxfId="33"/>
+    <tableColumn id="101" xr3:uid="{AFAA355A-5088-4D32-864A-D3766E3F2DB9}" name="Variable Current in X direction [mA]" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{B8B68D9B-B8A5-47C6-9E38-96ACC38FEEBF}" name="Variable Current in Y direction [mA]" dataDxfId="31"/>
+    <tableColumn id="113" xr3:uid="{52A1E8D6-8081-4659-A014-60E4EF5F0E59}" name="Conveyor density [g/cm³]" dataDxfId="30"/>
+    <tableColumn id="94" xr3:uid="{96888CAA-C7C5-4E47-8448-9191C49FA5A1}" name="Conveyor dimensions [cm³]" dataDxfId="29"/>
+    <tableColumn id="95" xr3:uid="{ED0D4D0E-1211-43F2-BC0E-22DA81926893}" name="Conveyor (X,Z,) offset to source [cm]²" dataDxfId="28"/>
+    <tableColumn id="98" xr3:uid="{A2FC2080-D096-4223-A065-59BF125992CF}" name="Conveyor speed [m/min]" dataDxfId="27"/>
+    <tableColumn id="99" xr3:uid="{5E6C370D-3088-4624-AFB4-003F396975BF}" name="Operation [hours/year]" dataDxfId="26"/>
+    <tableColumn id="102" xr3:uid="{770C3078-401F-4D26-A1DF-66B2FFE02E8B}" name="Central product density [g/cm³]" dataDxfId="25"/>
+    <tableColumn id="48" xr3:uid="{CCB69289-CD76-4BD9-9335-F57431C42E63}" name="Central product dimensions [cm³]" dataDxfId="24"/>
+    <tableColumn id="107" xr3:uid="{7D836FFB-FB1E-4F92-B391-5A079FD28583}" name="Central product (Y,Z,) position [cm]" dataDxfId="23"/>
+    <tableColumn id="105" xr3:uid="{52C3BF51-271E-47F7-AA33-2A718B0AF70E}" name="Central product resolution (X,Y,Z) [cm³]" dataDxfId="22"/>
+    <tableColumn id="80" xr3:uid="{9673494C-D662-4EC2-81E7-43A6012DBA29}" name="Central wooden pallet density [g/cm³]" dataDxfId="21"/>
+    <tableColumn id="78" xr3:uid="{AD143500-9222-4D71-A52F-89788F0E51BF}" name="Central wooden pallet dimensions [cm³]" dataDxfId="20"/>
+    <tableColumn id="104" xr3:uid="{64CF5341-FD0F-4CC6-8051-EDE54CCFDAFD}" name="Left product density [g/cm³]" dataDxfId="19"/>
+    <tableColumn id="103" xr3:uid="{302258E3-A3C1-449E-A147-45DF85CD8461}" name="Left product dimensions [cm³]" dataDxfId="18"/>
+    <tableColumn id="81" xr3:uid="{F4817E2A-8E0A-4F71-AEEF-983CB4BA5C5A}" name="Left product Y-gap [cm]" dataDxfId="17"/>
+    <tableColumn id="79" xr3:uid="{D4890004-1BD6-47CE-A0AD-30515FDE1C89}" name="Left wooden pallet density [g/cm³]" dataDxfId="16"/>
+    <tableColumn id="49" xr3:uid="{99EDCD1E-4E84-4177-8AE8-B85A1112E226}" name="Left wooden pallet dimensions [cm³]" dataDxfId="15"/>
+    <tableColumn id="68" xr3:uid="{134833D5-3CD0-445F-96A6-F83F3F601C27}" name="Right product density [g/cm³]" dataDxfId="14"/>
+    <tableColumn id="69" xr3:uid="{57F245DA-9F77-4C92-89BD-07EC51E62BA7}" name="Right product dimensions [cm³]" dataDxfId="13"/>
+    <tableColumn id="85" xr3:uid="{872D630E-21C6-45BA-BF05-CA39F0614DE6}" name="Right product Y-gap [cm]" dataDxfId="12"/>
+    <tableColumn id="84" xr3:uid="{65B9F3CC-FE71-4DC2-B3A1-DCE7E9DFB044}" name="Right wooden pallet density [g/cm³]" dataDxfId="11"/>
+    <tableColumn id="83" xr3:uid="{C788756D-428F-464B-BB5B-33F86DA3B670}" name="Right wooden pallet dimensions [cm³]" dataDxfId="10"/>
+    <tableColumn id="82" xr3:uid="{F993C600-89C0-4209-8324-76E491F0FF21}" name="Mother pallets density [g/cm³]" dataDxfId="9"/>
+    <tableColumn id="65" xr3:uid="{E2839587-C22B-4C24-A46E-35133C720E5D}" name="Mother pallets dimensions [cm³]" dataDxfId="8"/>
+    <tableColumn id="75" xr3:uid="{D92D691F-4F6B-4EA0-8A3B-CC42AE83D3EB}" name="Units (Gy/h) (kGy/h) (Gy) (kGy)" dataDxfId="7"/>
+    <tableColumn id="63" xr3:uid="{EF6E5902-20A7-42BC-AA8A-69AFA6FA6571}" name="Minimum dose" dataDxfId="6"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Purpose of the test" dataDxfId="5"/>
+    <tableColumn id="77" xr3:uid="{95DD1121-A20B-405B-B9A1-FE5D35E618A0}" name="List of n 0-D dose mapping points (X1,Y1,Z1), …, (Xn,Yn,Zn)" dataDxfId="4"/>
+    <tableColumn id="109" xr3:uid="{EAC4DB55-B00A-46BE-AD00-296DD033D394}" name="X-mapping (V or X)" dataDxfId="3"/>
+    <tableColumn id="111" xr3:uid="{738EFEBD-DE05-475E-AAEA-A33A35B3E948}" name="Y-mapping (V or X)" dataDxfId="2"/>
+    <tableColumn id="110" xr3:uid="{DBF499A0-44D0-419A-909B-771F65574919}" name="Z-mapping (V or X)" dataDxfId="1"/>
+    <tableColumn id="90" xr3:uid="{59CF94CA-802D-4A0C-8D11-1660040EBEDD}" name="List of p 1-D mapping points (X1,Y1,Z1), …, (Xp,Yp,Zp)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1847,8 +1874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:CK87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView zoomScale="97" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1926,16 +1953,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:89" ht="44" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="64" t="s">
+      <c r="B1" s="76"/>
+      <c r="C1" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
       <c r="G1" s="63"/>
       <c r="H1" s="36"/>
       <c r="I1" s="45" t="s">
@@ -1944,54 +1971,54 @@
       <c r="J1" s="45"/>
       <c r="K1" s="45"/>
       <c r="L1" s="46"/>
-      <c r="M1" s="64" t="s">
+      <c r="M1" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="66"/>
-      <c r="Q1" s="64" t="s">
+      <c r="N1" s="71"/>
+      <c r="O1" s="71"/>
+      <c r="P1" s="72"/>
+      <c r="Q1" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="R1" s="66"/>
-      <c r="S1" s="67" t="s">
+      <c r="R1" s="72"/>
+      <c r="S1" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="T1" s="68"/>
-      <c r="U1" s="69"/>
-      <c r="V1" s="64" t="s">
+      <c r="T1" s="74"/>
+      <c r="U1" s="75"/>
+      <c r="V1" s="70" t="s">
         <v>34</v>
       </c>
-      <c r="W1" s="66"/>
-      <c r="X1" s="67" t="s">
+      <c r="W1" s="72"/>
+      <c r="X1" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="Y1" s="68"/>
-      <c r="Z1" s="69"/>
-      <c r="AA1" s="64" t="s">
+      <c r="Y1" s="74"/>
+      <c r="Z1" s="75"/>
+      <c r="AA1" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="AB1" s="66"/>
-      <c r="AC1" s="67" t="s">
+      <c r="AB1" s="72"/>
+      <c r="AC1" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="AD1" s="69"/>
-      <c r="AE1" s="64" t="s">
+      <c r="AD1" s="75"/>
+      <c r="AE1" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="AF1" s="66"/>
+      <c r="AF1" s="72"/>
       <c r="AG1" s="53" t="s">
         <v>46</v>
       </c>
       <c r="AH1" s="53" t="s">
         <v>56</v>
       </c>
-      <c r="AI1" s="64" t="s">
+      <c r="AI1" s="70" t="s">
         <v>57</v>
       </c>
-      <c r="AJ1" s="65"/>
-      <c r="AK1" s="65"/>
-      <c r="AL1" s="66"/>
+      <c r="AJ1" s="71"/>
+      <c r="AK1" s="71"/>
+      <c r="AL1" s="72"/>
       <c r="AM1" s="5"/>
       <c r="AN1" s="5"/>
       <c r="AO1" s="5"/>
@@ -2042,7 +2069,7 @@
       <c r="E2" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="F2" s="73" t="s">
+      <c r="F2" s="66" t="s">
         <v>74</v>
       </c>
       <c r="G2" s="35" t="s">
@@ -2209,13 +2236,13 @@
       <c r="E3" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F3" s="71" t="s">
+      <c r="F3" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="G3" s="71" t="s">
+      <c r="G3" s="64" t="s">
         <v>76</v>
       </c>
-      <c r="H3" s="31" t="s">
+      <c r="H3" s="67" t="s">
         <v>65</v>
       </c>
       <c r="I3" s="12" t="s">
@@ -2325,13 +2352,13 @@
       <c r="E4" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F4" s="71" t="s">
+      <c r="F4" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="G4" s="71" t="s">
+      <c r="G4" s="64" t="s">
         <v>76</v>
       </c>
-      <c r="H4" s="31" t="s">
+      <c r="H4" s="67" t="s">
         <v>65</v>
       </c>
       <c r="I4" s="12" t="s">
@@ -2441,13 +2468,13 @@
       <c r="E5" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F5" s="71" t="s">
+      <c r="F5" s="64" t="s">
         <v>77</v>
       </c>
-      <c r="G5" s="71" t="s">
+      <c r="G5" s="64" t="s">
         <v>76</v>
       </c>
-      <c r="H5" s="31" t="s">
+      <c r="H5" s="69" t="s">
         <v>65</v>
       </c>
       <c r="I5" s="12" t="s">
@@ -2557,13 +2584,13 @@
       <c r="E6" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F6" s="71" t="s">
+      <c r="F6" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="G6" s="71" t="s">
+      <c r="G6" s="64" t="s">
         <v>76</v>
       </c>
-      <c r="H6" s="31" t="s">
+      <c r="H6" s="67" t="s">
         <v>65</v>
       </c>
       <c r="I6" s="12" t="s">
@@ -2673,13 +2700,13 @@
       <c r="E7" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F7" s="71" t="s">
+      <c r="F7" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="G7" s="71" t="s">
+      <c r="G7" s="64" t="s">
         <v>76</v>
       </c>
-      <c r="H7" s="31" t="s">
+      <c r="H7" s="69" t="s">
         <v>65</v>
       </c>
       <c r="I7" s="12" t="s">
@@ -2789,13 +2816,13 @@
       <c r="E8" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F8" s="71" t="s">
+      <c r="F8" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="G8" s="71" t="s">
+      <c r="G8" s="64" t="s">
         <v>76</v>
       </c>
-      <c r="H8" s="31" t="s">
+      <c r="H8" s="67" t="s">
         <v>65</v>
       </c>
       <c r="I8" s="12" t="s">
@@ -2905,13 +2932,13 @@
       <c r="E9" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F9" s="71" t="s">
+      <c r="F9" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="G9" s="71" t="s">
+      <c r="G9" s="64" t="s">
         <v>76</v>
       </c>
-      <c r="H9" s="31" t="s">
+      <c r="H9" s="67" t="s">
         <v>65</v>
       </c>
       <c r="I9" s="12" t="s">
@@ -3021,13 +3048,13 @@
       <c r="E10" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F10" s="71" t="s">
+      <c r="F10" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="G10" s="71" t="s">
+      <c r="G10" s="64" t="s">
         <v>76</v>
       </c>
-      <c r="H10" s="31" t="s">
+      <c r="H10" s="67" t="s">
         <v>65</v>
       </c>
       <c r="I10" s="12" t="s">
@@ -3137,13 +3164,13 @@
       <c r="E11" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="F11" s="72" t="s">
+      <c r="F11" s="65" t="s">
         <v>78</v>
       </c>
-      <c r="G11" s="72" t="s">
+      <c r="G11" s="65" t="s">
         <v>76</v>
       </c>
-      <c r="H11" s="33" t="s">
+      <c r="H11" s="68" t="s">
         <v>65</v>
       </c>
       <c r="I11" s="62" t="s">
@@ -4246,4 +4273,25 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4810C4A1-0AB6-4741-A7AB-7DD6371F3125}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="77" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="77"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>